<commit_message>
First draft of discussion.
</commit_message>
<xml_diff>
--- a/data/TEMPO_SR_2019-07-09.xlsx
+++ b/data/TEMPO_SR_2019-07-09.xlsx
@@ -8232,10 +8232,10 @@
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J53" sqref="J53"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>